<commit_message>
Fixed a bug that was causing the disable of the STTS751 timeout not to work.  Changed command interpreter to support 2 bytes of SCROD ID, which required moving SCROD Rev left by 1 byte as well.  See the data format page for details on the current format:  http://www.phys.hawaii.edu/~kurtisn/doku.php?id=itop:documentation:data_format&#data_packets_from_the_scrod
</commit_message>
<xml_diff>
--- a/USB_and_fiber_readout/firmware/FPGA/contrib/picoblaze_registers_and_memory.xlsx
+++ b/USB_and_fiber_readout/firmware/FPGA/contrib/picoblaze_registers_and_memory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Register</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Input values &amp; return values</t>
   </si>
   <si>
-    <t>Board stack revision (read at startup)</t>
-  </si>
-  <si>
-    <t>Board stack ID (read at startup)</t>
-  </si>
-  <si>
     <t>Packet_countdown(7:0)</t>
   </si>
   <si>
@@ -133,6 +127,21 @@
   </si>
   <si>
     <t>Write value [15:8]</t>
+  </si>
+  <si>
+    <t>Board stack ID low word (as read at startup from EEPROM address 00)</t>
+  </si>
+  <si>
+    <t>Board stack ID high word (as read at startup from EEPROM address 01)</t>
+  </si>
+  <si>
+    <t>Board stack revision (as read at startup from EEPROM address 02)</t>
+  </si>
+  <si>
+    <t>Reserved (but currently unused)</t>
+  </si>
+  <si>
+    <t>(after destination is verified, before that this is used for general workspace)</t>
   </si>
 </sst>
 </file>
@@ -491,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +600,10 @@
         <v>05</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -603,7 +615,10 @@
         <v>06</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -615,7 +630,7 @@
         <v>07</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -627,7 +642,7 @@
         <v>08</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -639,7 +654,7 @@
         <v>09</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -651,7 +666,7 @@
         <v>0A</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -663,7 +678,7 @@
         <v>0B</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -675,7 +690,7 @@
         <v>0C</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -687,7 +702,7 @@
         <v>0D</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -699,7 +714,7 @@
         <v>0E</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +749,7 @@
         <v>00</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +761,7 @@
         <v>01</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,7 +773,7 @@
         <v>02</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,7 +785,7 @@
         <v>03</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -782,7 +797,7 @@
         <v>04</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,7 +809,7 @@
         <v>05</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,7 +821,7 @@
         <v>06</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +833,7 @@
         <v>07</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,7 +845,7 @@
         <v>08</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,7 +857,7 @@
         <v>09</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -853,6 +868,9 @@
         <f t="shared" si="1"/>
         <v>0A</v>
       </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -862,6 +880,9 @@
         <f t="shared" si="1"/>
         <v>0B</v>
       </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -908,7 +929,7 @@
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,7 +965,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,10 +1022,10 @@
         <v>19</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,13 +1037,13 @@
         <v>1A</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s">
         <v>33</v>
-      </c>
-      <c r="F46" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1034,13 +1055,13 @@
         <v>1B</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" t="s">
         <v>34</v>
-      </c>
-      <c r="F47" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,13 +1073,13 @@
         <v>1C</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,13 +1091,13 @@
         <v>1D</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>